<commit_message>
Changed focus time for FRA_promise_econ_renewal and more work on defensive AI
</commit_message>
<xml_diff>
--- a/BiceE Documentation/FRA Historical Plan.xlsx
+++ b/BiceE Documentation/FRA Historical Plan.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\James Rankin\Documents\Paradox Interactive\Hearts of Iron IV\mod\BiceExpandedLocal\BiceE Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chimera\Documents\Paradox Interactive\Hearts of Iron IV\mod\BlackICE-Expanded\BiceE Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46FB6226-D141-4988-A3D0-06F1F6BD85D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AA6C8BF-373B-4AC3-9409-A99FC91D24AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28080" windowHeight="16440" xr2:uid="{4CEBE7C9-E6FE-4393-BB13-E322055FE4E0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28095" windowHeight="16440" xr2:uid="{4CEBE7C9-E6FE-4393-BB13-E322055FE4E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -710,8 +710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D5168CB-632A-4645-9810-F038E7CD2226}">
   <dimension ref="A1:D106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="A84" sqref="A84"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -755,11 +755,11 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="C4" s="1">
         <f>B1+B4</f>
-        <v>13164</v>
+        <v>13171</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -771,7 +771,7 @@
       </c>
       <c r="C5" s="1">
         <f>B5+C4</f>
-        <v>13185</v>
+        <v>13192</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -783,7 +783,7 @@
       </c>
       <c r="C6" s="1">
         <f t="shared" ref="C6:C13" si="0">B6+C5</f>
-        <v>13213</v>
+        <v>13220</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -795,7 +795,7 @@
       </c>
       <c r="C7" s="1">
         <f t="shared" si="0"/>
-        <v>13241</v>
+        <v>13248</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -803,11 +803,11 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="C8" s="1">
         <f t="shared" si="0"/>
-        <v>13269</v>
+        <v>13262</v>
       </c>
       <c r="D8" t="s">
         <v>11</v>
@@ -822,7 +822,7 @@
       </c>
       <c r="C9" s="1">
         <f t="shared" si="0"/>
-        <v>13402</v>
+        <v>13395</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -834,7 +834,7 @@
       </c>
       <c r="C10" s="1">
         <f t="shared" si="0"/>
-        <v>13416</v>
+        <v>13409</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -846,7 +846,7 @@
       </c>
       <c r="C11" s="1">
         <f t="shared" si="0"/>
-        <v>13437</v>
+        <v>13430</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -858,7 +858,7 @@
       </c>
       <c r="C12" s="1">
         <f t="shared" si="0"/>
-        <v>13465</v>
+        <v>13458</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -870,7 +870,7 @@
       </c>
       <c r="C13" s="1">
         <f t="shared" si="0"/>
-        <v>13493</v>
+        <v>13486</v>
       </c>
       <c r="D13" t="s">
         <v>12</v>
@@ -885,7 +885,7 @@
       </c>
       <c r="C14" s="1">
         <f t="shared" ref="C14:C45" si="1">B14+C13</f>
-        <v>13507</v>
+        <v>13500</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -897,7 +897,7 @@
       </c>
       <c r="C15" s="1">
         <f t="shared" si="1"/>
-        <v>13535</v>
+        <v>13528</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -909,7 +909,7 @@
       </c>
       <c r="C16" s="1">
         <f t="shared" si="1"/>
-        <v>13563</v>
+        <v>13556</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -921,7 +921,7 @@
       </c>
       <c r="C17" s="1">
         <f t="shared" si="1"/>
-        <v>13703</v>
+        <v>13696</v>
       </c>
       <c r="D17" t="s">
         <v>22</v>
@@ -936,7 +936,7 @@
       </c>
       <c r="C18" s="1">
         <f t="shared" si="1"/>
-        <v>13717</v>
+        <v>13710</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -948,7 +948,7 @@
       </c>
       <c r="C19" s="1">
         <f t="shared" si="1"/>
-        <v>13738</v>
+        <v>13731</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -960,7 +960,7 @@
       </c>
       <c r="C20" s="1">
         <f t="shared" si="1"/>
-        <v>13766</v>
+        <v>13759</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -972,7 +972,7 @@
       </c>
       <c r="C21" s="1">
         <f t="shared" si="1"/>
-        <v>13794</v>
+        <v>13787</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -984,7 +984,7 @@
       </c>
       <c r="C22" s="5">
         <f t="shared" si="1"/>
-        <v>13822</v>
+        <v>13815</v>
       </c>
       <c r="D22" s="4"/>
     </row>
@@ -997,7 +997,7 @@
       </c>
       <c r="C23" s="1">
         <f t="shared" si="1"/>
-        <v>13850</v>
+        <v>13843</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1009,7 +1009,7 @@
       </c>
       <c r="C24" s="1">
         <f t="shared" si="1"/>
-        <v>13864</v>
+        <v>13857</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1021,7 +1021,7 @@
       </c>
       <c r="C25" s="1">
         <f t="shared" si="1"/>
-        <v>13892</v>
+        <v>13885</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1033,7 +1033,7 @@
       </c>
       <c r="C26" s="1">
         <f t="shared" si="1"/>
-        <v>13913</v>
+        <v>13906</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1045,7 +1045,7 @@
       </c>
       <c r="C27" s="1">
         <f t="shared" si="1"/>
-        <v>13934</v>
+        <v>13927</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1057,7 +1057,7 @@
       </c>
       <c r="C28" s="1">
         <f t="shared" si="1"/>
-        <v>13962</v>
+        <v>13955</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1069,7 +1069,7 @@
       </c>
       <c r="C29" s="1">
         <f t="shared" si="1"/>
-        <v>13990</v>
+        <v>13983</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1081,7 +1081,7 @@
       </c>
       <c r="C30" s="1">
         <f t="shared" si="1"/>
-        <v>14018</v>
+        <v>14011</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1093,7 +1093,7 @@
       </c>
       <c r="C31" s="1">
         <f t="shared" si="1"/>
-        <v>14039</v>
+        <v>14032</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1105,7 +1105,7 @@
       </c>
       <c r="C32" s="1">
         <f t="shared" si="1"/>
-        <v>14067</v>
+        <v>14060</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -1117,7 +1117,7 @@
       </c>
       <c r="C33" s="1">
         <f t="shared" si="1"/>
-        <v>14095</v>
+        <v>14088</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -1129,7 +1129,7 @@
       </c>
       <c r="C34" s="1">
         <f t="shared" si="1"/>
-        <v>14123</v>
+        <v>14116</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -1141,7 +1141,7 @@
       </c>
       <c r="C35" s="1">
         <f t="shared" si="1"/>
-        <v>14137</v>
+        <v>14130</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -1153,7 +1153,7 @@
       </c>
       <c r="C36" s="1">
         <f t="shared" si="1"/>
-        <v>14158</v>
+        <v>14151</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -1165,7 +1165,7 @@
       </c>
       <c r="C37" s="1">
         <f t="shared" si="1"/>
-        <v>14179</v>
+        <v>14172</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -1177,7 +1177,7 @@
       </c>
       <c r="C38" s="1">
         <f t="shared" si="1"/>
-        <v>14200</v>
+        <v>14193</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -1189,7 +1189,7 @@
       </c>
       <c r="C39" s="1">
         <f t="shared" si="1"/>
-        <v>14221</v>
+        <v>14214</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -1201,7 +1201,7 @@
       </c>
       <c r="C40" s="1">
         <f t="shared" si="1"/>
-        <v>14242</v>
+        <v>14235</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -1213,7 +1213,7 @@
       </c>
       <c r="C41" s="1">
         <f t="shared" si="1"/>
-        <v>14270</v>
+        <v>14263</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -1225,7 +1225,7 @@
       </c>
       <c r="C42" s="1">
         <f t="shared" si="1"/>
-        <v>14298</v>
+        <v>14291</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -1237,7 +1237,7 @@
       </c>
       <c r="C43" s="1">
         <f t="shared" si="1"/>
-        <v>14326</v>
+        <v>14319</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -1249,7 +1249,7 @@
       </c>
       <c r="C44" s="1">
         <f t="shared" si="1"/>
-        <v>14354</v>
+        <v>14347</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -1261,7 +1261,7 @@
       </c>
       <c r="C45" s="1">
         <f t="shared" si="1"/>
-        <v>14382</v>
+        <v>14375</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -1273,7 +1273,7 @@
       </c>
       <c r="C46" s="1">
         <f t="shared" ref="C46:C66" si="2">B46+C45</f>
-        <v>14396</v>
+        <v>14389</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -1285,7 +1285,7 @@
       </c>
       <c r="C47" s="1">
         <f t="shared" si="2"/>
-        <v>14438</v>
+        <v>14431</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -1297,7 +1297,7 @@
       </c>
       <c r="C48" s="1">
         <f t="shared" si="2"/>
-        <v>14466</v>
+        <v>14459</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -1309,7 +1309,7 @@
       </c>
       <c r="C49" s="1">
         <f t="shared" si="2"/>
-        <v>14494</v>
+        <v>14487</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -1321,7 +1321,7 @@
       </c>
       <c r="C50" s="1">
         <f t="shared" si="2"/>
-        <v>14501</v>
+        <v>14494</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -1333,7 +1333,7 @@
       </c>
       <c r="C51" s="1">
         <f t="shared" si="2"/>
-        <v>14529</v>
+        <v>14522</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -1345,7 +1345,7 @@
       </c>
       <c r="C52" s="1">
         <f t="shared" si="2"/>
-        <v>14550</v>
+        <v>14543</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -1357,7 +1357,7 @@
       </c>
       <c r="C53" s="1">
         <f t="shared" si="2"/>
-        <v>14571</v>
+        <v>14564</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -1369,7 +1369,7 @@
       </c>
       <c r="C54" s="1">
         <f t="shared" si="2"/>
-        <v>14592</v>
+        <v>14585</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -1381,7 +1381,7 @@
       </c>
       <c r="C55" s="1">
         <f t="shared" si="2"/>
-        <v>14620</v>
+        <v>14613</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -1393,7 +1393,7 @@
       </c>
       <c r="C56" s="1">
         <f t="shared" si="2"/>
-        <v>14648</v>
+        <v>14641</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -1405,7 +1405,7 @@
       </c>
       <c r="C57" s="1">
         <f t="shared" si="2"/>
-        <v>14676</v>
+        <v>14669</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -1417,7 +1417,7 @@
       </c>
       <c r="C58" s="1">
         <f t="shared" si="2"/>
-        <v>14690</v>
+        <v>14683</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -1429,7 +1429,7 @@
       </c>
       <c r="C59" s="1">
         <f t="shared" si="2"/>
-        <v>14718</v>
+        <v>14711</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -1441,7 +1441,7 @@
       </c>
       <c r="C60" s="1">
         <f t="shared" si="2"/>
-        <v>14746</v>
+        <v>14739</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -1453,7 +1453,7 @@
       </c>
       <c r="C61" s="1">
         <f t="shared" si="2"/>
-        <v>14774</v>
+        <v>14767</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -1465,7 +1465,7 @@
       </c>
       <c r="C62" s="1">
         <f t="shared" si="2"/>
-        <v>14802</v>
+        <v>14795</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -1477,7 +1477,7 @@
       </c>
       <c r="C63" s="1">
         <f t="shared" si="2"/>
-        <v>14830</v>
+        <v>14823</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -1489,7 +1489,7 @@
       </c>
       <c r="C64" s="1">
         <f t="shared" si="2"/>
-        <v>14858</v>
+        <v>14851</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -1501,7 +1501,7 @@
       </c>
       <c r="C65" s="1">
         <f t="shared" si="2"/>
-        <v>14886</v>
+        <v>14879</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -1513,7 +1513,7 @@
       </c>
       <c r="C66" s="1">
         <f t="shared" si="2"/>
-        <v>14914</v>
+        <v>14907</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -1525,7 +1525,7 @@
       </c>
       <c r="C67" s="1">
         <f t="shared" ref="C67:C106" si="3">B67+C66</f>
-        <v>14942</v>
+        <v>14935</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -1537,7 +1537,7 @@
       </c>
       <c r="C68" s="1">
         <f t="shared" si="3"/>
-        <v>14970</v>
+        <v>14963</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -1549,7 +1549,7 @@
       </c>
       <c r="C69" s="1">
         <f t="shared" si="3"/>
-        <v>14998</v>
+        <v>14991</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -1561,7 +1561,7 @@
       </c>
       <c r="C70" s="1">
         <f t="shared" si="3"/>
-        <v>15026</v>
+        <v>15019</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -1573,7 +1573,7 @@
       </c>
       <c r="C71" s="1">
         <f t="shared" si="3"/>
-        <v>15054</v>
+        <v>15047</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -1585,7 +1585,7 @@
       </c>
       <c r="C72" s="1">
         <f t="shared" si="3"/>
-        <v>15082</v>
+        <v>15075</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -1597,7 +1597,7 @@
       </c>
       <c r="C73" s="1">
         <f t="shared" si="3"/>
-        <v>15110</v>
+        <v>15103</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -1609,7 +1609,7 @@
       </c>
       <c r="C74" s="1">
         <f t="shared" si="3"/>
-        <v>15138</v>
+        <v>15131</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -1621,7 +1621,7 @@
       </c>
       <c r="C75" s="1">
         <f t="shared" si="3"/>
-        <v>15166</v>
+        <v>15159</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -1633,7 +1633,7 @@
       </c>
       <c r="C76" s="1">
         <f t="shared" si="3"/>
-        <v>15194</v>
+        <v>15187</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -1645,7 +1645,7 @@
       </c>
       <c r="C77" s="1">
         <f t="shared" si="3"/>
-        <v>15222</v>
+        <v>15215</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -1657,7 +1657,7 @@
       </c>
       <c r="C78" s="1">
         <f t="shared" si="3"/>
-        <v>15257</v>
+        <v>15250</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -1669,7 +1669,7 @@
       </c>
       <c r="C79" s="1">
         <f t="shared" si="3"/>
-        <v>15285</v>
+        <v>15278</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
@@ -1681,7 +1681,7 @@
       </c>
       <c r="C80" s="1">
         <f t="shared" si="3"/>
-        <v>15313</v>
+        <v>15306</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
@@ -1693,7 +1693,7 @@
       </c>
       <c r="C81" s="1">
         <f t="shared" si="3"/>
-        <v>15341</v>
+        <v>15334</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
@@ -1705,7 +1705,7 @@
       </c>
       <c r="C82" s="1">
         <f t="shared" si="3"/>
-        <v>15369</v>
+        <v>15362</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
@@ -1717,145 +1717,145 @@
       </c>
       <c r="C83" s="1">
         <f t="shared" si="3"/>
-        <v>15397</v>
+        <v>15390</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C84" s="1">
         <f t="shared" si="3"/>
-        <v>15397</v>
+        <v>15390</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C85" s="1">
         <f t="shared" si="3"/>
-        <v>15397</v>
+        <v>15390</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C86" s="1">
         <f t="shared" si="3"/>
-        <v>15397</v>
+        <v>15390</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C87" s="1">
         <f t="shared" si="3"/>
-        <v>15397</v>
+        <v>15390</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C88" s="1">
         <f t="shared" si="3"/>
-        <v>15397</v>
+        <v>15390</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C89" s="1">
         <f t="shared" si="3"/>
-        <v>15397</v>
+        <v>15390</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C90" s="1">
         <f t="shared" si="3"/>
-        <v>15397</v>
+        <v>15390</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C91" s="1">
         <f t="shared" si="3"/>
-        <v>15397</v>
+        <v>15390</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C92" s="1">
         <f t="shared" si="3"/>
-        <v>15397</v>
+        <v>15390</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C93" s="1">
         <f t="shared" si="3"/>
-        <v>15397</v>
+        <v>15390</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C94" s="1">
         <f t="shared" si="3"/>
-        <v>15397</v>
+        <v>15390</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C95" s="1">
         <f t="shared" si="3"/>
-        <v>15397</v>
+        <v>15390</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C96" s="1">
         <f t="shared" si="3"/>
-        <v>15397</v>
+        <v>15390</v>
       </c>
     </row>
     <row r="97" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C97" s="1">
         <f t="shared" si="3"/>
-        <v>15397</v>
+        <v>15390</v>
       </c>
     </row>
     <row r="98" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C98" s="1">
         <f t="shared" si="3"/>
-        <v>15397</v>
+        <v>15390</v>
       </c>
     </row>
     <row r="99" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C99" s="1">
         <f t="shared" si="3"/>
-        <v>15397</v>
+        <v>15390</v>
       </c>
     </row>
     <row r="100" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C100" s="1">
         <f t="shared" si="3"/>
-        <v>15397</v>
+        <v>15390</v>
       </c>
     </row>
     <row r="101" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C101" s="1">
         <f t="shared" si="3"/>
-        <v>15397</v>
+        <v>15390</v>
       </c>
     </row>
     <row r="102" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C102" s="1">
         <f t="shared" si="3"/>
-        <v>15397</v>
+        <v>15390</v>
       </c>
     </row>
     <row r="103" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C103" s="1">
         <f t="shared" si="3"/>
-        <v>15397</v>
+        <v>15390</v>
       </c>
     </row>
     <row r="104" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C104" s="1">
         <f t="shared" si="3"/>
-        <v>15397</v>
+        <v>15390</v>
       </c>
     </row>
     <row r="105" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C105" s="1">
         <f t="shared" si="3"/>
-        <v>15397</v>
+        <v>15390</v>
       </c>
     </row>
     <row r="106" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C106" s="1">
         <f t="shared" si="3"/>
-        <v>15397</v>
+        <v>15390</v>
       </c>
     </row>
   </sheetData>

</xml_diff>